<commit_message>
For RQ1 & RQ2, all 120 responses are used
</commit_message>
<xml_diff>
--- a/dataset/combined_analysis.xlsx
+++ b/dataset/combined_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADEBB11F-349C-3342-AB08-E4B2240DB433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F073FAD-A381-CD43-B59A-AE3E0E13F36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1140" windowWidth="30240" windowHeight="17300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All RQ" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>ChatGPT has four varying levels of confidence in its responses. When ChatGPT is "highly confident" in its response, we find that its answers or explanations are correct about half the time. On the other hand, when ChatGPT is "confident" in its response, we find that its answers or explanation are twice as likely to be correct than incorrect.</t>
   </si>
@@ -180,18 +180,6 @@
     <t>Percentage of incorrect</t>
   </si>
   <si>
-    <t>separate_1</t>
-  </si>
-  <si>
-    <t>Total asked questions (Separate Context)</t>
-  </si>
-  <si>
-    <t>separate_2</t>
-  </si>
-  <si>
-    <t>separate_3</t>
-  </si>
-  <si>
     <t>Inconsistance Percentage</t>
   </si>
   <si>
@@ -243,6 +231,9 @@
     <t>answers are inconsistent 16.1% and 32.5% of the time in shared and separate context queries.
 For explanation, inconsistency rates are 19.4% and 32.5% in the shared and separate contexts
 shared context queries produce fewer inconsistencies in terms of both answers and explanations. Overall, ChatGPT’s explanations and answers are quite nondeterministic across multiple iterations.</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -358,7 +349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -381,12 +372,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -439,6 +439,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5197,10 +5201,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5514,10 +5514,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="141" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5525,10 +5525,10 @@
     </row>
     <row r="3" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5536,10 +5536,10 @@
     </row>
     <row r="5" spans="1:3" ht="101" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5547,7 +5547,7 @@
     </row>
     <row r="7" spans="1:3" ht="88" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>0</v>
@@ -6096,10 +6096,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6158,7 +6158,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="8">
         <v>2</v>
@@ -6182,11 +6182,11 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="K2" s="16">
         <f t="shared" ref="K2:K4" si="0">SUM(B2:J2)</f>
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
@@ -6194,7 +6194,7 @@
       </c>
       <c r="N2" s="8">
         <f>SUM(B2:J4)</f>
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -6204,10 +6204,10 @@
         <v>41</v>
       </c>
       <c r="B3" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -6228,11 +6228,11 @@
         <v>0</v>
       </c>
       <c r="J3" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="K3" s="16">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
@@ -6240,7 +6240,7 @@
       </c>
       <c r="N3" s="8">
         <f>SUM(C2:D4,F2:I4)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -6250,10 +6250,10 @@
         <v>43</v>
       </c>
       <c r="B4" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="8">
         <v>0</v>
@@ -6274,27 +6274,113 @@
         <v>1</v>
       </c>
       <c r="J4" s="1">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K4" s="16">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <f>SUM(B2:B4)</f>
+        <v>42</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:K5" si="1">SUM(C2:C4)</f>
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="8" t="s">
         <v>44</v>
       </c>
       <c r="N5" s="12">
         <f>N3/N2</f>
-        <v>0.11827956989247312</v>
+        <v>0.10833333333333334</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="13">
+        <f>B5/$K$5</f>
+        <v>0.35</v>
+      </c>
+      <c r="C6" s="13">
+        <f t="shared" ref="C6:K6" si="2">C5/$K$5</f>
+        <v>0.05</v>
+      </c>
+      <c r="D6" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" si="2"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="I6" s="13">
+        <f t="shared" si="2"/>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="J6" s="13">
+        <f t="shared" si="2"/>
+        <v>0.49166666666666664</v>
+      </c>
+      <c r="K6" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6304,219 +6390,38 @@
       </c>
       <c r="N7" s="13">
         <f>SUM(J2:J4)/N2</f>
-        <v>0.43010752688172044</v>
+        <v>0.49166666666666664</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <f>SUM(D2:D4,G2:G4)</f>
-        <v>4</v>
-      </c>
-      <c r="C8" s="22">
-        <f>(B8+B26)/ (N2+N21)</f>
-        <v>1.8779342723004695E-2</v>
-      </c>
+      <c r="B8" s="27">
+        <f>SUM(B6,E6,J6)</f>
+        <v>0.89166666666666661</v>
+      </c>
+      <c r="C8" s="22"/>
       <c r="M8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="N8" s="13">
         <f>SUM(B2:B4)/N2</f>
-        <v>0.38709677419354838</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="E9" s="22">
-        <f>SUM(C2:C4,F2:F4,C21:C23,F21:F23) / (N2+N21)</f>
-        <v>6.5727699530516437E-2</v>
-      </c>
+      <c r="E9" s="22"/>
     </row>
-    <row r="20" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>6</v>
-      </c>
+    <row r="20" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="M20" s="8"/>
+      <c r="N20" s="12"/>
     </row>
-    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="1">
-        <v>14</v>
-      </c>
-      <c r="C21" s="8">
-        <v>5</v>
-      </c>
-      <c r="D21" s="8">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <v>3</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0</v>
-      </c>
-      <c r="G21" s="8">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="8">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
-        <v>18</v>
-      </c>
-      <c r="K21" s="16">
-        <f>SUM(B21:J21)</f>
-        <v>40</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N21" s="8">
-        <f>SUM(B21:J23)</f>
-        <v>120</v>
-      </c>
+    <row r="22" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="13"/>
     </row>
-    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="1">
-        <v>14</v>
-      </c>
-      <c r="C22" s="8">
-        <v>3</v>
-      </c>
-      <c r="D22" s="8">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2</v>
-      </c>
-      <c r="F22" s="8">
-        <v>0</v>
-      </c>
-      <c r="G22" s="8">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1">
-        <v>1</v>
-      </c>
-      <c r="I22" s="8">
-        <v>1</v>
-      </c>
-      <c r="J22" s="1">
-        <v>19</v>
-      </c>
-      <c r="K22" s="16">
-        <f>SUM(B22:J22)</f>
-        <v>40</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N22" s="8">
-        <f>SUM(C21:D23,F21:I23)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="1">
-        <v>13</v>
-      </c>
-      <c r="C23" s="8">
-        <v>2</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
-        <v>2</v>
-      </c>
-      <c r="F23" s="8">
-        <v>0</v>
-      </c>
-      <c r="G23" s="8">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="8">
-        <v>2</v>
-      </c>
-      <c r="J23" s="1">
-        <v>21</v>
-      </c>
-      <c r="K23" s="16">
-        <f>SUM(B23:J23)</f>
-        <v>40</v>
-      </c>
+    <row r="23" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="M24" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="N24" s="12">
-        <f>N22/N21</f>
-        <v>0.11666666666666667</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B26" s="5">
-        <f>SUM(D21:D23,G21:G23)</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N26" s="13">
-        <f>SUM(J21:J23)/N21</f>
-        <v>0.48333333333333334</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="M27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N27" s="13">
-        <f>SUM(B21:B23)/N21</f>
-        <v>0.34166666666666667</v>
-      </c>
+      <c r="N23" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6527,8 +6432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -6539,7 +6444,7 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C2" s="25"/>
       <c r="F2" s="24"/>
@@ -6547,10 +6452,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -6558,39 +6463,31 @@
         <v>7</v>
       </c>
       <c r="B4" s="18">
-        <f>5/31</f>
-        <v>0.16129032258064516</v>
+        <f>6/40</f>
+        <v>0.15</v>
       </c>
       <c r="C4" s="18">
-        <f>6/31</f>
-        <v>0.19354838709677419</v>
+        <f>7/40</f>
+        <v>0.17499999999999999</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="13">
-        <f>13/40</f>
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="C5" s="13">
-        <f>13/40</f>
-        <v>0.32500000000000001</v>
-      </c>
+      <c r="A5" s="14"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -6606,7 +6503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E26E6D-7A63-0640-A728-10E012F3926A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -6629,7 +6526,7 @@
     </row>
     <row r="2" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2" s="19">
         <v>8</v>
@@ -6643,7 +6540,7 @@
     </row>
     <row r="3" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B3" s="19">
         <v>3</v>
@@ -6657,7 +6554,7 @@
     </row>
     <row r="4" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B4" s="19">
         <v>8</v>
@@ -6671,7 +6568,7 @@
     </row>
     <row r="5" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B5" s="19">
         <v>1</v>
@@ -6690,7 +6587,7 @@
     </row>
     <row r="11" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B11" s="19">
         <v>9</v>
@@ -6704,7 +6601,7 @@
     </row>
     <row r="12" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B12" s="19">
         <v>3</v>
@@ -6718,7 +6615,7 @@
     </row>
     <row r="13" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B13" s="19">
         <v>9</v>
@@ -6729,7 +6626,7 @@
     </row>
     <row r="14" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B14" s="19">
         <v>1</v>

</xml_diff>

<commit_message>
Results are organized for public release.
</commit_message>
<xml_diff>
--- a/dataset/combined_analysis.xlsx
+++ b/dataset/combined_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F073FAD-A381-CD43-B59A-AE3E0E13F36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54BCA3D-D1E9-1B4E-8C69-6022E9BEDE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1140" windowWidth="30240" windowHeight="17300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All RQ" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
   <si>
     <t>ChatGPT has four varying levels of confidence in its responses. When ChatGPT is "highly confident" in its response, we find that its answers or explanations are correct about half the time. On the other hand, when ChatGPT is "confident" in its response, we find that its answers or explanation are twice as likely to be correct than incorrect.</t>
   </si>
@@ -180,6 +180,18 @@
     <t>Percentage of incorrect</t>
   </si>
   <si>
+    <t>separate_1</t>
+  </si>
+  <si>
+    <t>Total asked questions (Separate Context)</t>
+  </si>
+  <si>
+    <t>separate_2</t>
+  </si>
+  <si>
+    <t>separate_3</t>
+  </si>
+  <si>
     <t>Inconsistance Percentage</t>
   </si>
   <si>
@@ -233,7 +245,7 @@
 shared context queries produce fewer inconsistencies in terms of both answers and explanations. Overall, ChatGPT’s explanations and answers are quite nondeterministic across multiple iterations.</t>
   </si>
   <si>
-    <t>%</t>
+    <t xml:space="preserve">Sum </t>
   </si>
 </sst>
 </file>
@@ -435,14 +447,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1704,8 +1716,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.3866879563906065E-2"/>
-          <c:y val="9.5091170076159026E-2"/>
+          <c:x val="9.2769646088505492E-2"/>
+          <c:y val="3.9535433070866134E-2"/>
           <c:w val="0.91226624087218788"/>
           <c:h val="0.74517119450647928"/>
         </c:manualLayout>
@@ -1795,7 +1807,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1914,8 +1926,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.3473063966577662E-2"/>
-                  <c:y val="-4.0034679027730619E-17"/>
+                  <c:x val="2.5317829397629974E-2"/>
+                  <c:y val="-1.3102409949302958E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1928,6 +1940,27 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-80D2-9349-82A9-A481808EA327}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.0776172844738459E-3"/>
+                  <c:y val="8.7349399662019732E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-F50E-264C-8C7A-52906B0E6CCC}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1945,7 +1978,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2056,7 +2089,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2085,7 +2118,18 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2101,7 +2145,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2127,10 +2171,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.7146844143834381"/>
-          <c:y val="0.18967922136607585"/>
+          <c:x val="0.71468430252195814"/>
+          <c:y val="0.11106476167025808"/>
           <c:w val="0.24458564325268042"/>
-          <c:h val="0.14100703540952081"/>
+          <c:h val="0.10606727554471292"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2146,7 +2190,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2200,10 +2244,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.3939412048520185E-2"/>
-          <c:y val="0.12072837396897715"/>
-          <c:w val="0.9121211759029596"/>
-          <c:h val="0.70234906760868732"/>
+          <c:x val="9.2664324217537328E-2"/>
+          <c:y val="5.4821959755030618E-2"/>
+          <c:w val="0.90733567578246266"/>
+          <c:h val="0.73340183892107824"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2230,19 +2274,20 @@
             </a:solidFill>
             <a:ln>
               <a:noFill/>
-              <a:prstDash val="solid"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="1"/>
+              <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.3966952026465555E-2"/>
-                  <c:y val="0"/>
+                  <c:x val="-1.2218963831867057E-2"/>
+                  <c:y val="8.7351502445842076E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -2252,18 +2297,19 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-4D25-1940-8F43-4E77E63413B2}"/>
+                  <c16:uniqueId val="{00000002-24DC-0942-9D28-9EB67F2D29D3}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="2"/>
+              <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.796144403087648E-2"/>
-                  <c:y val="-8.0444933104008947E-17"/>
+                  <c:x val="-1.6291951775822745E-2"/>
+                  <c:y val="-4.3675751222921238E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -2273,7 +2319,29 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-4D25-1940-8F43-4E77E63413B2}"/>
+                  <c16:uniqueId val="{00000004-24DC-0942-9D28-9EB67F2D29D3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6291951775822745E-2"/>
+                  <c:y val="4.3675751222921038E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-24DC-0942-9D28-9EB67F2D29D3}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2281,8 +2349,8 @@
               <a:noFill/>
               <a:ln>
                 <a:noFill/>
-                <a:prstDash val="solid"/>
               </a:ln>
+              <a:effectLst/>
             </c:spPr>
             <c:txPr>
               <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -2291,7 +2359,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2306,6 +2374,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -2315,7 +2384,21 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -2356,7 +2439,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B9CA-6D4E-B676-798F952FD866}"/>
+              <c16:uniqueId val="{00000000-24DC-0942-9D28-9EB67F2D29D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2380,8 +2463,8 @@
             </a:solidFill>
             <a:ln>
               <a:noFill/>
-              <a:prstDash val="solid"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -2389,10 +2472,11 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.1955936035287368E-2"/>
-                  <c:y val="8.7759122629899045E-3"/>
+                  <c:x val="1.6291951775822745E-2"/>
+                  <c:y val="-2.0017821396257851E-17"/>
                 </c:manualLayout>
               </c:layout>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -2402,28 +2486,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-4D25-1940-8F43-4E77E63413B2}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.997246002205463E-2"/>
-                  <c:y val="-8.0444933104008947E-17"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-4D25-1940-8F43-4E77E63413B2}"/>
+                  <c16:uniqueId val="{00000003-24DC-0942-9D28-9EB67F2D29D3}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2431,8 +2494,8 @@
               <a:noFill/>
               <a:ln>
                 <a:noFill/>
-                <a:prstDash val="solid"/>
               </a:ln>
+              <a:effectLst/>
             </c:spPr>
             <c:txPr>
               <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -2441,7 +2504,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2456,6 +2519,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -2465,7 +2529,21 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -2506,13 +2584,14 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B9CA-6D4E-B676-798F952FD866}"/>
+              <c16:uniqueId val="{00000001-24DC-0942-9D28-9EB67F2D29D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2520,18 +2599,18 @@
         </c:dLbls>
         <c:gapWidth val="350"/>
         <c:overlap val="-27"/>
-        <c:axId val="249312095"/>
-        <c:axId val="734263631"/>
+        <c:axId val="1850916528"/>
+        <c:axId val="1874545488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="249312095"/>
+        <c:axId val="1850916528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -2543,16 +2622,16 @@
                 <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:prstDash val="solid"/>
             <a:round/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
           <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2567,7 +2646,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="734263631"/>
+        <c:crossAx val="1874545488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2575,7 +2654,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="734263631"/>
+        <c:axId val="1874545488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2584,29 +2663,34 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
             <a:noFill/>
-            <a:prstDash val="solid"/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
           <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2621,37 +2705,44 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249312095"/>
+        <c:crossAx val="1850916528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72658425641745017"/>
-          <c:y val="0.20005452121870471"/>
-          <c:w val="0.2414598075472624"/>
-          <c:h val="0.13226612712081667"/>
+          <c:x val="0.68844272031978404"/>
+          <c:y val="0.1322230971128609"/>
+          <c:w val="0.26257334585376241"/>
+          <c:h val="0.13559667541557305"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="1"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
-          <a:prstDash val="solid"/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
       <c:txPr>
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2672,10 +2763,25 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:ln>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
+      <a:round/>
     </a:ln>
+    <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -2744,7 +2850,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2873,7 +2979,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -2999,7 +3105,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3095,7 +3201,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="150"/>
         <c:overlap val="-27"/>
         <c:axId val="746029791"/>
         <c:axId val="439011455"/>
@@ -3129,7 +3235,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3188,7 +3294,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3221,8 +3327,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.76981007946538338"/>
-          <c:y val="0.19044947851550101"/>
+          <c:x val="0.76981011537780653"/>
+          <c:y val="0.13803841540247722"/>
           <c:w val="0.13232993007235144"/>
           <c:h val="0.17088277017423292"/>
         </c:manualLayout>
@@ -3240,7 +3346,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3348,7 +3454,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3477,7 +3583,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3603,7 +3709,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3696,7 +3802,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="150"/>
         <c:overlap val="-27"/>
         <c:axId val="566392815"/>
         <c:axId val="1192896543"/>
@@ -3730,7 +3836,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3789,7 +3895,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3807,6 +3913,7 @@
         <c:crossAx val="566392815"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3822,8 +3929,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.78392092198849794"/>
-          <c:y val="0.17312036508054793"/>
+          <c:x val="0.78392093400348417"/>
+          <c:y val="0.14691491000731827"/>
           <c:w val="0.13781040338257428"/>
           <c:h val="0.17391694334738128"/>
         </c:manualLayout>
@@ -3841,7 +3948,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3969,6 +4076,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4473,6 +4620,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5059,8 +5709,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>954689</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>166414</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>70069</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5087,23 +5737,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1156139</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>153715</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>950309</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>213711</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>402933</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>171163</xdr:rowOff>
+      <xdr:colOff>827723</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>134884</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9400740-B911-5AFC-D28F-BEA62E4BE93E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5135,9 +5785,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>55880</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>252815</xdr:rowOff>
+      <xdr:colOff>19304</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5171,9 +5821,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>43180</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>127931</xdr:rowOff>
+      <xdr:colOff>6604</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5514,10 +6164,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="141" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5525,10 +6175,10 @@
     </row>
     <row r="3" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5536,10 +6186,10 @@
     </row>
     <row r="5" spans="1:3" ht="101" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5547,7 +6197,7 @@
     </row>
     <row r="7" spans="1:3" ht="88" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>0</v>
@@ -5575,8 +6225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -5584,7 +6234,8 @@
     <col min="1" max="1" width="13.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="16.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" style="1" customWidth="1"/>
@@ -6096,10 +6747,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6158,7 +6809,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8">
         <v>2</v>
@@ -6182,11 +6833,11 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="K2" s="16">
         <f t="shared" ref="K2:K4" si="0">SUM(B2:J2)</f>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
@@ -6194,7 +6845,7 @@
       </c>
       <c r="N2" s="8">
         <f>SUM(B2:J4)</f>
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -6204,10 +6855,10 @@
         <v>41</v>
       </c>
       <c r="B3" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -6228,11 +6879,11 @@
         <v>0</v>
       </c>
       <c r="J3" s="1">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="K3" s="16">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
@@ -6240,7 +6891,7 @@
       </c>
       <c r="N3" s="8">
         <f>SUM(C2:D4,F2:I4)</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -6250,10 +6901,10 @@
         <v>43</v>
       </c>
       <c r="B4" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="8">
         <v>0</v>
@@ -6274,59 +6925,55 @@
         <v>1</v>
       </c>
       <c r="J4" s="1">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="K4" s="16">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5">
         <f>SUM(B2:B4)</f>
-        <v>42</v>
-      </c>
-      <c r="C5" s="1">
-        <f t="shared" ref="C5:K5" si="1">SUM(C2:C4)</f>
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
+        <v>36</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:J5" si="1">SUM(C2:C4)</f>
+        <v>4</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5">
         <f t="shared" si="1"/>
-        <v>59</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="8" t="s">
@@ -6334,52 +6981,45 @@
       </c>
       <c r="N5" s="12">
         <f>N3/N2</f>
-        <v>0.10833333333333334</v>
+        <v>0.11827956989247312</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="13">
-        <f>B5/$K$5</f>
-        <v>0.35</v>
-      </c>
-      <c r="C6" s="13">
-        <f t="shared" ref="C6:K6" si="2">C5/$K$5</f>
-        <v>0.05</v>
-      </c>
-      <c r="D6" s="13">
+      <c r="B6" s="22">
+        <f>B5/SUM($K$2:$K$4)</f>
+        <v>0.38709677419354838</v>
+      </c>
+      <c r="C6" s="22">
+        <f t="shared" ref="C6:J6" si="2">C5/SUM($K$2:$K$4)</f>
+        <v>4.3010752688172046E-2</v>
+      </c>
+      <c r="D6" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="22">
         <f t="shared" si="2"/>
-        <v>0.05</v>
-      </c>
-      <c r="F6" s="13">
+        <v>6.4516129032258063E-2</v>
+      </c>
+      <c r="F6" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="22">
         <f t="shared" si="2"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="H6" s="13">
+        <v>4.3010752688172046E-2</v>
+      </c>
+      <c r="H6" s="22">
         <f t="shared" si="2"/>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="I6" s="13">
+        <v>2.1505376344086023E-2</v>
+      </c>
+      <c r="I6" s="22">
         <f t="shared" si="2"/>
-        <v>8.3333333333333332E-3</v>
-      </c>
-      <c r="J6" s="13">
+        <v>1.0752688172043012E-2</v>
+      </c>
+      <c r="J6" s="22">
         <f t="shared" si="2"/>
-        <v>0.49166666666666664</v>
-      </c>
-      <c r="K6" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.43010752688172044</v>
       </c>
       <c r="L6" s="1"/>
     </row>
@@ -6390,38 +7030,225 @@
       </c>
       <c r="N7" s="13">
         <f>SUM(J2:J4)/N2</f>
-        <v>0.49166666666666664</v>
+        <v>0.43010752688172044</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="27">
-        <f>SUM(B6,E6,J6)</f>
-        <v>0.89166666666666661</v>
-      </c>
-      <c r="C8" s="22"/>
+      <c r="B8">
+        <f>SUM(D2:D4,G2:G4)</f>
+        <v>4</v>
+      </c>
+      <c r="C8" s="22">
+        <f>(B8+B26)/ (N2+N21)</f>
+        <v>1.8779342723004695E-2</v>
+      </c>
       <c r="M8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="N8" s="13">
         <f>SUM(B2:B4)/N2</f>
-        <v>0.35</v>
+        <v>0.38709677419354838</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="E9" s="22"/>
+      <c r="E9" s="22">
+        <f>SUM(C2:C4,F2:F4,C21:C23,F21:F23) / (N2+N21)</f>
+        <v>6.5727699530516437E-2</v>
+      </c>
     </row>
-    <row r="20" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="M20" s="8"/>
-      <c r="N20" s="12"/>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="25">
+        <f>SUM(B6,E6,J6)</f>
+        <v>0.88172043010752688</v>
+      </c>
     </row>
-    <row r="22" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="13"/>
+    <row r="20" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="1">
+        <v>14</v>
+      </c>
+      <c r="C21" s="8">
+        <v>5</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>18</v>
+      </c>
+      <c r="K21" s="16">
+        <f>SUM(B21:J21)</f>
+        <v>40</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N21" s="8">
+        <f>SUM(B21:J23)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1">
+        <v>14</v>
+      </c>
+      <c r="C22" s="8">
+        <v>3</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="8">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>19</v>
+      </c>
+      <c r="K22" s="16">
+        <f>SUM(B22:J22)</f>
+        <v>40</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N22" s="8">
+        <f>SUM(C21:D23,F21:I23)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="1">
+        <v>13</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="8">
+        <v>2</v>
+      </c>
+      <c r="J23" s="1">
+        <v>21</v>
+      </c>
+      <c r="K23" s="16">
+        <f>SUM(B23:J23)</f>
+        <v>40</v>
+      </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="13"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="M24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="N24" s="12">
+        <f>N22/N21</f>
+        <v>0.11666666666666667</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
+        <f>SUM(D21:D23,G21:G23)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N26" s="13">
+        <f>SUM(J21:J23)/N21</f>
+        <v>0.48333333333333334</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="M27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N27" s="13">
+        <f>SUM(B21:B23)/N21</f>
+        <v>0.34166666666666667</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6432,8 +7259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -6443,19 +7270,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
+      <c r="B2" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -6463,31 +7290,39 @@
         <v>7</v>
       </c>
       <c r="B4" s="18">
-        <f>6/40</f>
-        <v>0.15</v>
+        <f>5/31</f>
+        <v>0.16129032258064516</v>
       </c>
       <c r="C4" s="18">
-        <f>7/40</f>
-        <v>0.17499999999999999</v>
+        <f>6/31</f>
+        <v>0.19354838709677419</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="A5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="13">
+        <f>13/40</f>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="C5" s="13">
+        <f>13/40</f>
+        <v>0.32500000000000001</v>
+      </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -6504,7 +7339,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -6526,7 +7361,7 @@
     </row>
     <row r="2" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B2" s="19">
         <v>8</v>
@@ -6540,7 +7375,7 @@
     </row>
     <row r="3" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B3" s="19">
         <v>3</v>
@@ -6554,7 +7389,7 @@
     </row>
     <row r="4" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B4" s="19">
         <v>8</v>
@@ -6568,7 +7403,7 @@
     </row>
     <row r="5" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B5" s="19">
         <v>1</v>
@@ -6587,7 +7422,7 @@
     </row>
     <row r="11" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B11" s="19">
         <v>9</v>
@@ -6601,7 +7436,7 @@
     </row>
     <row r="12" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B12" s="19">
         <v>3</v>
@@ -6615,7 +7450,7 @@
     </row>
     <row r="13" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B13" s="19">
         <v>9</v>
@@ -6626,7 +7461,7 @@
     </row>
     <row r="14" spans="1:4" ht="22" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B14" s="19">
         <v>1</v>

</xml_diff>

<commit_message>
Fixed result calculation in combined_analysis.xlsx
</commit_message>
<xml_diff>
--- a/dataset/combined_analysis.xlsx
+++ b/dataset/combined_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF285E15-5170-7E4A-B681-E25D3DE0AF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CCB6DC-E169-074A-92D0-70F97DA6F4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-200" yWindow="11220" windowWidth="30240" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
@@ -347,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -405,6 +405,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,25 +583,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00">
-                  <c:v>12.333333333333334</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>11</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -710,25 +713,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>12.666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -846,13 +849,13 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00">
-                  <c:v>3.6666666666666665</c:v>
+                  <c:v>3.3333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3</c:v>
@@ -1321,25 +1324,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.333333333333334</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1451,25 +1454,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>1.6666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1701,6 +1704,48 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.631046913789546E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-AB4C-774F-AF09-DFEEEA10F5F5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.4465703706843225E-2"/>
+                  <c:y val="5.5555555555555558E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-3B5D-1544-BAF3-1A6550D13225}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1752,10 +1797,10 @@
                   <c:v>Correct (EC)</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Partially Correct (EPC)</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Incorrect (EIC)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Partially Correct (EPC)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1767,13 +1812,13 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.39784946236559143</c:v>
+                  <c:v>0.40740740740740738</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4838709677419355</c:v>
+                  <c:v>0.1234567901234568</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11827956989247311</c:v>
+                  <c:v>0.46913580246913578</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1809,6 +1854,48 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.6310469137895311E-2"/>
+                  <c:y val="1.1111111111111009E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-AB4C-774F-AF09-DFEEEA10F5F5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.6310469137895234E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-3B5D-1544-BAF3-1A6550D13225}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1860,10 +1947,10 @@
                   <c:v>Correct (EC)</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Partially Correct (EPC)</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Incorrect (EIC)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Partially Correct (EPC)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1875,13 +1962,13 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.34408602150537632</c:v>
+                  <c:v>0.32098765432098764</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54838709677419351</c:v>
+                  <c:v>0.1111111111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10752688172043011</c:v>
+                  <c:v>0.5679012345679012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2017,8 +2104,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.71468430252195814"/>
-          <c:y val="0.1110647616702581"/>
+          <c:x val="0.47818250002247514"/>
+          <c:y val="4.4398075240594921E-2"/>
           <c:w val="0.2445856432526804"/>
           <c:h val="0.1060672755447129"/>
         </c:manualLayout>
@@ -2056,6 +2143,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -2120,6 +2212,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6291951775822745E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-144B-2543-9CD1-A189A5299B7C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2172,10 +2286,10 @@
                   <c:v>Correct (AC)</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Partially Correct (APC)</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Incorrect (AIC)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Partially Correct (APC)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2187,13 +2301,13 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.33333333333333337</c:v>
+                  <c:v>0.49382716049382719</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35833333333333334</c:v>
+                  <c:v>6.1728395061728399E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.3333333333333343E-2</c:v>
+                  <c:v>0.44444444444444442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2229,6 +2343,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.6291951775822745E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-144B-2543-9CD1-A189A5299B7C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2281,10 +2417,10 @@
                   <c:v>Correct (AC)</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Partially Correct (APC)</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Incorrect (AIC)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Partially Correct (APC)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2296,13 +2432,13 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.23333333333333334</c:v>
+                  <c:v>0.30107526881720431</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43333333333333329</c:v>
+                  <c:v>6.4516129032258063E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10833333333333332</c:v>
+                  <c:v>0.5053763440860215</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2441,8 +2577,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.68844272031978404"/>
-          <c:y val="0.1322230971128609"/>
+          <c:x val="0.4481364316263986"/>
+          <c:y val="6.5556430446194233E-2"/>
           <c:w val="0.26257334585376241"/>
           <c:h val="0.13559667541557299"/>
         </c:manualLayout>
@@ -2480,6 +2616,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -2604,13 +2745,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -2633,7 +2774,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>EIC</c:v>
+                  <c:v>EPC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2719,13 +2860,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2745,7 +2886,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>EPC</c:v>
+                  <c:v>EIC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3139,13 +3280,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -3165,6 +3306,114 @@
           <c:tx>
             <c:strRef>
               <c:f>'RQ4'!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>APC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RQ4'!$A$11:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Highly confident</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Very confident</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Confident</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Reliable</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RQ4'!$C$11:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7CF3-994D-95D6-9D732021CCFE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RQ4'!$D$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3249,127 +3498,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RQ4'!$C$11:$C$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7CF3-994D-95D6-9D732021CCFE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'RQ4'!$D$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>APC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'RQ4'!$A$11:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Highly confident</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Very confident</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Confident</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Reliable</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>'RQ4'!$D$11:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4081,8 +4221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A14" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -4127,8 +4267,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <f>4*6</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -4145,7 +4284,7 @@
       </c>
       <c r="G2" s="1">
         <f>SUM(B2:F2)</f>
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -4153,23 +4292,23 @@
         <v>7</v>
       </c>
       <c r="B3" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
       </c>
       <c r="G3" s="1">
         <f>SUM(B3:F3)</f>
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4210,38 +4349,38 @@
         <v>17</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="17">
         <f>AVERAGE(B8:D8)</f>
-        <v>12.333333333333334</v>
+        <v>11</v>
       </c>
       <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
         <v>9</v>
       </c>
-      <c r="G8">
-        <v>11</v>
-      </c>
       <c r="H8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I8" s="17">
         <f>AVERAGE(F8:H8)</f>
-        <v>10.666666666666666</v>
+        <v>8.6666666666666661</v>
       </c>
       <c r="J8" s="17">
         <f>AVERAGE(B8:D8,F8:H8)</f>
-        <v>11.5</v>
+        <v>9.8333333333333339</v>
       </c>
       <c r="K8" s="12">
         <f>J8/$G$2</f>
-        <v>0.37096774193548387</v>
+        <v>0.36419753086419754</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -4249,38 +4388,38 @@
         <v>18</v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E9" s="17">
         <f>AVERAGE(B9:D9)</f>
+        <v>12.666666666666666</v>
+      </c>
+      <c r="F9">
+        <v>17</v>
+      </c>
+      <c r="G9">
         <v>15</v>
       </c>
-      <c r="F9">
-        <v>18</v>
-      </c>
-      <c r="G9">
-        <v>17</v>
-      </c>
       <c r="H9">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I9" s="17">
         <f>AVERAGE(F9:H9)</f>
-        <v>17</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="J9" s="17">
         <f>AVERAGE(B9:D9,F9:H9)</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K9" s="12">
         <f>J9/$G$2</f>
-        <v>0.5161290322580645</v>
+        <v>0.51851851851851849</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -4294,14 +4433,14 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="17">
         <f>AVERAGE(B10:D10)</f>
-        <v>3.6666666666666665</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -4311,15 +4450,15 @@
       </c>
       <c r="I10" s="17">
         <f>AVERAGE(F10:H10)</f>
-        <v>3.3333333333333335</v>
+        <v>3</v>
       </c>
       <c r="J10" s="17">
         <f>AVERAGE(B10:D10,F10:H10)</f>
-        <v>3.5</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="K10" s="12">
         <f>J10/$G$2</f>
-        <v>0.11290322580645161</v>
+        <v>0.11728395061728394</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -4410,7 +4549,7 @@
       </c>
       <c r="K18" s="12">
         <f>J18/$G$2</f>
-        <v>0.36559139784946237</v>
+        <v>0.41975308641975312</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -4418,38 +4557,38 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C19">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D19">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E19" s="1">
         <f>AVERAGE(B19:D19)</f>
-        <v>14.333333333333334</v>
+        <v>12</v>
       </c>
       <c r="F19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G19">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H19">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I19" s="17">
         <f>AVERAGE(F19:H19)</f>
-        <v>17.333333333333332</v>
+        <v>15.666666666666666</v>
       </c>
       <c r="J19" s="17">
         <f>AVERAGE(B19:D19,F19:H19)</f>
-        <v>15.833333333333334</v>
+        <v>13.833333333333334</v>
       </c>
       <c r="K19" s="12">
         <f>J19/$G$2</f>
-        <v>0.510752688172043</v>
+        <v>0.51234567901234573</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -4457,38 +4596,38 @@
         <v>22</v>
       </c>
       <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
         <v>2</v>
       </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
       <c r="D20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1">
         <f>AVERAGE(B20:D20)</f>
-        <v>3.3333333333333335</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I20" s="17">
         <f>AVERAGE(F20:H20)</f>
-        <v>4.333333333333333</v>
+        <v>2</v>
       </c>
       <c r="J20" s="17">
         <f>AVERAGE(B20:D20,F20:H20)</f>
-        <v>3.8333333333333335</v>
+        <v>1.8333333333333333</v>
       </c>
       <c r="K20" s="12">
         <f>J20/$G$2</f>
-        <v>0.12365591397849462</v>
+        <v>6.7901234567901231E-2</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -4509,90 +4648,90 @@
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="13">
+      <c r="B40" s="18">
         <f>E8/$G$2</f>
-        <v>0.39784946236559143</v>
+        <v>0.40740740740740738</v>
       </c>
       <c r="C40" s="13">
         <f>I8/$G$2</f>
-        <v>0.34408602150537632</v>
+        <v>0.32098765432098764</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F40" s="18">
-        <f>E18/$G$3</f>
-        <v>0.33333333333333337</v>
+        <f>E18/$G$2</f>
+        <v>0.49382716049382719</v>
       </c>
       <c r="G40" s="13">
         <f>I18/$G$3</f>
-        <v>0.23333333333333334</v>
+        <v>0.30107526881720431</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="13">
-        <f>E9/$G$2</f>
-        <v>0.4838709677419355</v>
-      </c>
-      <c r="C41" s="18">
-        <f>I9/$G$2</f>
-        <v>0.54838709677419351</v>
+        <v>27</v>
+      </c>
+      <c r="B41" s="18">
+        <f>E10/$G$2</f>
+        <v>0.1234567901234568</v>
+      </c>
+      <c r="C41" s="13">
+        <f>I10/$G$2</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F41" s="18">
-        <f>E19/$G$3</f>
-        <v>0.35833333333333334</v>
+        <f>E20/$G$2</f>
+        <v>6.1728395061728399E-2</v>
       </c>
       <c r="G41" s="13">
-        <f>I19/$G$3</f>
-        <v>0.43333333333333329</v>
+        <f>I20/$G$3</f>
+        <v>6.4516129032258063E-2</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B42" s="13">
-        <f>E10/$G$2</f>
-        <v>0.11827956989247311</v>
+        <f>E9/$G$2</f>
+        <v>0.46913580246913578</v>
       </c>
       <c r="C42" s="18">
-        <f>I10/$G$2</f>
-        <v>0.10752688172043011</v>
+        <f>I9/$G$2</f>
+        <v>0.5679012345679012</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F42" s="13">
-        <f>E20/$G$3</f>
-        <v>8.3333333333333343E-2</v>
-      </c>
-      <c r="G42" s="13">
-        <f>I20/$G$3</f>
-        <v>0.10833333333333332</v>
+        <f>E19/$G$2</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G42" s="18">
+        <f>I19/$G$3</f>
+        <v>0.5053763440860215</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="22">
         <f>B40+B42</f>
-        <v>0.5161290322580645</v>
+        <v>0.87654320987654311</v>
       </c>
       <c r="C44" s="22">
         <f>C40+C42</f>
-        <v>0.45161290322580644</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="F44" s="22">
         <f>F40+F42</f>
-        <v>0.41666666666666674</v>
+        <v>0.93827160493827155</v>
       </c>
       <c r="G44" s="22">
         <f>G40+G42</f>
-        <v>0.34166666666666667</v>
+        <v>0.80645161290322576</v>
       </c>
     </row>
   </sheetData>
@@ -4605,8 +4744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4665,7 +4804,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="1">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8">
         <v>2</v>
@@ -4686,14 +4825,14 @@
         <v>0</v>
       </c>
       <c r="I2" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K2" s="16">
         <f>SUM(B2:J2)</f>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
@@ -4701,7 +4840,7 @@
       </c>
       <c r="N2" s="8">
         <f>SUM(B2:J4)</f>
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -4711,7 +4850,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" s="8">
         <v>1</v>
@@ -4720,7 +4859,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" s="8">
         <v>0</v>
@@ -4732,14 +4871,14 @@
         <v>0</v>
       </c>
       <c r="I3" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K3" s="16">
         <f>SUM(B3:J3)</f>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
@@ -4747,7 +4886,7 @@
       </c>
       <c r="N3" s="8">
         <f>SUM(C2:D4,F2:I4)</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -4757,7 +4896,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
@@ -4766,7 +4905,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -4778,14 +4917,14 @@
         <v>1</v>
       </c>
       <c r="I4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" s="16">
         <f>SUM(B4:J4)</f>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -4797,7 +4936,7 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" ref="B5:J5" si="0">SUM(B2:B4)</f>
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
@@ -4809,7 +4948,7 @@
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
@@ -4825,11 +4964,11 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -4838,17 +4977,17 @@
       </c>
       <c r="N5" s="12">
         <f>N3/N2</f>
-        <v>0.125</v>
+        <v>0.11827956989247312</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13">
         <f t="shared" ref="B6:J6" si="1">B5/SUM($K$2:$K$4)</f>
-        <v>0.4</v>
+        <v>0.34408602150537637</v>
       </c>
       <c r="C6" s="13">
         <f t="shared" si="1"/>
-        <v>3.3333333333333333E-2</v>
+        <v>4.3010752688172046E-2</v>
       </c>
       <c r="D6" s="13">
         <f t="shared" si="1"/>
@@ -4856,7 +4995,7 @@
       </c>
       <c r="E6" s="13">
         <f t="shared" si="1"/>
-        <v>6.6666666666666666E-2</v>
+        <v>5.3763440860215055E-2</v>
       </c>
       <c r="F6" s="13">
         <f t="shared" si="1"/>
@@ -4864,19 +5003,19 @@
       </c>
       <c r="G6" s="13">
         <f t="shared" si="1"/>
-        <v>0.05</v>
+        <v>6.4516129032258063E-2</v>
       </c>
       <c r="H6" s="13">
         <f t="shared" si="1"/>
-        <v>8.3333333333333332E-3</v>
+        <v>1.0752688172043012E-2</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" si="1"/>
-        <v>3.3333333333333333E-2</v>
+        <v>0</v>
       </c>
       <c r="J6" s="13">
         <f t="shared" si="1"/>
-        <v>0.40833333333333333</v>
+        <v>0.4838709677419355</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -4888,7 +5027,7 @@
       </c>
       <c r="N7" s="13">
         <f>SUM(J2:J4)/N2</f>
-        <v>0.40833333333333333</v>
+        <v>0.4838709677419355</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4898,13 +5037,21 @@
       </c>
       <c r="N8" s="13">
         <f>SUM(B2:B4)/N2</f>
-        <v>0.4</v>
+        <v>0.34408602150537637</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C9" s="25">
+        <f>SUM(B6,E6,J6)</f>
+        <v>0.88172043010752699</v>
+      </c>
       <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="F10" s="25">
+        <f>SUM(B6:J6)</f>
+        <v>1</v>
+      </c>
       <c r="N10" s="24"/>
       <c r="O10" s="25"/>
     </row>
@@ -4921,7 +5068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -4952,12 +5099,12 @@
         <v>6</v>
       </c>
       <c r="B4" s="18">
-        <f>5/40</f>
-        <v>0.125</v>
+        <f>3/31</f>
+        <v>9.6774193548387094E-2</v>
       </c>
       <c r="C4" s="18">
-        <f>4/40</f>
-        <v>0.1</v>
+        <f>2/31</f>
+        <v>6.4516129032258063E-2</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
@@ -4978,10 +5125,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -4991,32 +5138,32 @@
     <col min="12" max="16384" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="19">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>52</v>
       </c>
@@ -5030,21 +5177,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>54</v>
       </c>
@@ -5052,7 +5199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
@@ -5060,60 +5207,58 @@
       <c r="C6" s="26"/>
       <c r="D6" s="26">
         <f>SUM(B2:D5)</f>
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="20" t="s">
-        <v>22</v>
-      </c>
+      <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="19">
+        <v>7</v>
+      </c>
+      <c r="C11" s="19">
+        <v>1</v>
+      </c>
+      <c r="D11" s="19">
         <v>8</v>
       </c>
-      <c r="C11" s="19">
-        <v>11</v>
-      </c>
-      <c r="D11" s="19">
-        <v>1</v>
-      </c>
     </row>
-    <row r="12" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B12" s="19">
         <v>3</v>
       </c>
-      <c r="C12" s="19">
+      <c r="D12" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="19">
-        <v>7</v>
-      </c>
-      <c r="C13" s="19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>54</v>
       </c>
@@ -5121,7 +5266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>5</v>
       </c>
@@ -5129,7 +5274,7 @@
       <c r="C15" s="26"/>
       <c r="D15" s="26">
         <f>SUM(B11:D14)</f>
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added dataset with 40 questions.xlsx
</commit_message>
<xml_diff>
--- a/dataset/combined_analysis.xlsx
+++ b/dataset/combined_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F450260D-5A61-6445-A6FB-D12BCBABA658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CE6E7D-585D-4D46-A951-0ED3BF7379B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
@@ -1726,8 +1726,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.4465703706843225E-2"/>
-                  <c:y val="5.5555555555555558E-3"/>
+                  <c:x val="-1.6310469137895384E-2"/>
+                  <c:y val="-5.5555555555555558E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1759,10 +1759,7 @@
                 <a:pPr>
                   <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="accent1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1852,6 +1849,27 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.6310469137895384E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-9873-1B41-A943-169ED82D115B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
@@ -1876,7 +1894,7 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.6310469137895234E-2"/>
+                  <c:x val="8.1552345689476918E-3"/>
                   <c:y val="0"/>
                 </c:manualLayout>
               </c:layout>
@@ -1909,10 +1927,7 @@
                 <a:pPr>
                   <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="accent2"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2210,6 +2225,28 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.1459758879114472E-3"/>
+                  <c:y val="-1.6666666666666666E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-EC9F-B043-AA50-BCD62C149CF3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
@@ -2247,10 +2284,7 @@
                 <a:pPr>
                   <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="accent1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2378,10 +2412,7 @@
                 <a:pPr>
                   <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="accent2"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2688,9 +2719,120 @@
                 <a:pPr>
                   <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RQ4'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Highly confident</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Very confident</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Confident</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Reliable</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RQ4'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E643-FF4C-A66D-07C8BBD0D27D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RQ4'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EPC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -2737,41 +2879,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RQ4'!$B$2:$B$5</c:f>
+              <c:f>'RQ4'!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E643-FF4C-A66D-07C8BBD0D27D}"/>
+              <c16:uniqueId val="{00000001-E643-FF4C-A66D-07C8BBD0D27D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'RQ4'!$C$1</c:f>
+              <c:f>'RQ4'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>EPC</c:v>
+                  <c:v>EIC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2803,10 +2945,7 @@
                 <a:pPr>
                   <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="accent2"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2852,7 +2991,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'RQ4'!$C$2:$C$5</c:f>
+              <c:f>'RQ4'!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2865,117 +3004,8 @@
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E643-FF4C-A66D-07C8BBD0D27D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'RQ4'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>EIC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'RQ4'!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Highly confident</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Very confident</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Confident</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>Reliable</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'RQ4'!$D$2:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3153,6 +3183,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -3223,10 +3258,7 @@
                 <a:pPr>
                   <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="accent1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3340,9 +3372,8 @@
                 <a:pPr>
                   <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -3396,6 +3427,15 @@
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3446,10 +3486,7 @@
                 <a:pPr>
                   <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="accent2"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3507,6 +3544,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3685,6 +3725,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -4218,8 +4263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -4742,7 +4787,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5125,7 +5170,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -5154,10 +5199,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="19">
+        <v>1</v>
+      </c>
+      <c r="D2" s="19">
         <v>10</v>
-      </c>
-      <c r="D2" s="19">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
@@ -5168,10 +5213,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="19">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19">
         <v>2</v>
-      </c>
-      <c r="D3" s="19">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
@@ -5194,6 +5239,12 @@
       </c>
       <c r="B5" s="19">
         <v>1</v>
+      </c>
+      <c r="C5" s="19">
+        <v>0</v>
+      </c>
+      <c r="D5" s="19">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">
@@ -5239,6 +5290,9 @@
       <c r="B12" s="19">
         <v>3</v>
       </c>
+      <c r="C12" s="19">
+        <v>0</v>
+      </c>
       <c r="D12" s="19">
         <v>3</v>
       </c>
@@ -5250,6 +5304,9 @@
       <c r="B13" s="19">
         <v>6</v>
       </c>
+      <c r="C13" s="19">
+        <v>0</v>
+      </c>
       <c r="D13" s="19">
         <v>2</v>
       </c>
@@ -5260,6 +5317,12 @@
       </c>
       <c r="B14" s="19">
         <v>1</v>
+      </c>
+      <c r="C14" s="19">
+        <v>0</v>
+      </c>
+      <c r="D14" s="19">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated README.md and cleaned dataset.
</commit_message>
<xml_diff>
--- a/dataset/combined_analysis.xlsx
+++ b/dataset/combined_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E022369-73A5-E84C-9B36-13A8D2C62B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF323AE-607A-454A-989A-6850D74B8BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1667,7 +1667,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="9.2769646088505492E-2"/>
-          <c:y val="3.9535433070866127E-2"/>
+          <c:y val="7.2604466108403112E-2"/>
           <c:w val="0.91226624087218788"/>
           <c:h val="0.74517119450647928"/>
         </c:manualLayout>
@@ -1706,7 +1706,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-1.631046913789546E-2"/>
-                  <c:y val="0"/>
+                  <c:y val="1.984126984126984E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1894,8 +1894,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="8.1552345689476918E-3"/>
-                  <c:y val="0"/>
+                  <c:x val="0"/>
+                  <c:y val="-6.6137566137566134E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -2116,10 +2116,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.47818250002247514"/>
-          <c:y val="4.4398075240594921E-2"/>
+          <c:x val="0.46594964816905354"/>
+          <c:y val="7.7466879140107484E-2"/>
           <c:w val="0.2445856432526804"/>
-          <c:h val="0.16559128025663458"/>
+          <c:h val="0.1259087405740949"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2190,7 +2190,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="9.2664324217537328E-2"/>
-          <c:y val="5.4821959755030618E-2"/>
+          <c:y val="8.7890576177977756E-2"/>
           <c:w val="0.90733567578246266"/>
           <c:h val="0.73340183892107824"/>
         </c:manualLayout>
@@ -2250,8 +2250,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.6291951775822745E-2"/>
-                  <c:y val="0"/>
+                  <c:x val="-1.6291951775822894E-2"/>
+                  <c:y val="-3.968253968253968E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="outEnd"/>
@@ -2375,11 +2375,33 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.2218963831867021E-2"/>
+                  <c:y val="3.3068783068783067E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-A4F4-264E-A32B-3DC414CB8D47}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.6291951775822745E-2"/>
-                  <c:y val="0"/>
+                  <c:x val="4.0729879439556863E-3"/>
+                  <c:y val="-1.5156350485738086E-17"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="outEnd"/>
@@ -2605,10 +2627,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.4481364316263986"/>
-          <c:y val="6.5556430446194233E-2"/>
+          <c:x val="0.49293929900991112"/>
+          <c:y val="8.5397658626005082E-2"/>
           <c:w val="0.26257334585376241"/>
-          <c:h val="0.13559667541557299"/>
+          <c:h val="0.11575532225138524"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2703,6 +2725,72 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8617920016641144E-17"/>
+                  <c:y val="2.6031671525399525E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-0004-2149-85CB-1F84EE3FC5C9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.6127660321316158E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-0004-2149-85CB-1F84EE3FC5C9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.9523753644049686E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-0004-2149-85CB-1F84EE3FC5C9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2805,16 +2893,92 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:pattFill prst="wdDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent3"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.9523753644049686E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-0004-2149-85CB-1F84EE3FC5C9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.9523753644049686E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-0004-2149-85CB-1F84EE3FC5C9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.4471680066564575E-17"/>
+                  <c:y val="1.9523753644049686E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-0004-2149-85CB-1F84EE3FC5C9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2929,6 +3093,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.9523753644049686E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-0004-2149-85CB-1F84EE3FC5C9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -3144,10 +3330,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.76981011537780653"/>
-          <c:y val="0.13803841540247719"/>
-          <c:w val="0.13232993007235139"/>
-          <c:h val="0.1708827701742329"/>
+          <c:x val="0.73717464558680679"/>
+          <c:y val="0.13144821204579341"/>
+          <c:w val="0.16496540514843344"/>
+          <c:h val="0.20345775378355335"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3163,7 +3349,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3242,6 +3428,72 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8617920016641144E-17"/>
+                  <c:y val="1.315147024635189E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-60D0-F448-BCDE-4E7F76E47329}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.315147024635189E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-60D0-F448-BCDE-4E7F76E47329}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.315147024635189E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-60D0-F448-BCDE-4E7F76E47329}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -3344,18 +3596,50 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:pattFill prst="wdDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.315147024635189E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-60D0-F448-BCDE-4E7F76E47329}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -3470,6 +3754,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.315147024635189E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-60D0-F448-BCDE-4E7F76E47329}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -3686,10 +3992,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.78392093400348417"/>
-          <c:y val="0.14691491000731829"/>
-          <c:w val="0.1378104033825743"/>
-          <c:h val="0.17391694334738131"/>
+          <c:x val="0.74312677910082936"/>
+          <c:y val="0.1600297588701467"/>
+          <c:w val="0.17860483492763027"/>
+          <c:h val="0.21971997887605138"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3705,7 +4011,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="800" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3814,16 +4120,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>178677</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>148896</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>336333</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>183931</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>954689</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>770759</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>229826</xdr:rowOff>
+      <xdr:rowOff>2102</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3853,13 +4159,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>950309</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>213711</xdr:rowOff>
+      <xdr:rowOff>178676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>827723</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>31882</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>259606</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3891,16 +4197,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>366805</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>226358</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19304</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>78740</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>265205</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>20469</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3927,16 +4233,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>490818</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>6604</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>197273</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>389218</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>107626</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4263,8 +4569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A21" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -4778,6 +5084,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -5103,6 +5410,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5162,6 +5470,7 @@
     <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5169,8 +5478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -5338,6 +5647,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>